<commit_message>
workflow - job build in github hoster runner
</commit_message>
<xml_diff>
--- a/doc/Road_To_Pro.xlsx
+++ b/doc/Road_To_Pro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC51549E-CA39-4788-B6A7-8BB7ECCEB103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE5C1B2-6FE9-4D62-9EC5-7990D5A1DFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="131">
   <si>
     <t>Topic</t>
   </si>
@@ -419,13 +419,16 @@
   </si>
   <si>
     <t>Etiquetado de recursos para atribución de costes.</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,8 +444,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +483,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -483,10 +498,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -500,15 +516,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -518,8 +525,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -800,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E29"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -834,7 +854,7 @@
       <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -845,7 +865,7 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -854,7 +874,7 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -863,7 +883,7 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -872,7 +892,7 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
@@ -881,7 +901,7 @@
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -890,7 +910,7 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -899,21 +919,21 @@
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -922,14 +942,14 @@
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -938,7 +958,7 @@
       <c r="C15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
@@ -947,7 +967,7 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
@@ -956,7 +976,7 @@
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -967,7 +987,7 @@
       <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
@@ -976,7 +996,7 @@
       <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
@@ -985,7 +1005,7 @@
       <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
@@ -994,7 +1014,7 @@
       <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
@@ -1003,7 +1023,7 @@
       <c r="C22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
@@ -1012,7 +1032,7 @@
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
@@ -1021,54 +1041,54 @@
       <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1085,17 +1105,17 @@
   <dimension ref="B2:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="42.21875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="42.21875" style="7" customWidth="1"/>
     <col min="4" max="4" width="78.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15" style="10" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="5" max="5" width="15" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -1116,784 +1136,788 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="8"/>
+      <c r="E3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>1.2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="8"/>
+      <c r="E4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>2.1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="8"/>
+      <c r="E6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="E7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
+      <c r="B8" s="6">
         <v>2.4</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="8"/>
+      <c r="E8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
+      <c r="B9" s="6">
         <v>3.1</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="8"/>
+      <c r="E9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>3.2</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="8"/>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <v>3.3</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="8"/>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
+      <c r="B12" s="6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="8"/>
+      <c r="E12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>5.2</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="8"/>
+      <c r="E13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>5.3</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="8"/>
+      <c r="E14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <v>6.1</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="8"/>
+      <c r="E15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="9">
+      <c r="B16" s="6">
         <v>6.2</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="8"/>
+      <c r="E16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
+      <c r="B17" s="6">
         <v>6.3</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="8"/>
+      <c r="E17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="9">
+      <c r="B18" s="6">
         <v>7.1</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="8"/>
+      <c r="E18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="9">
+      <c r="B19" s="6">
         <v>7.2</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="8"/>
+      <c r="E19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="9">
+      <c r="B20" s="6">
         <v>9.1</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="8"/>
+      <c r="E20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="9">
+      <c r="B21" s="6">
         <v>10.1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="8"/>
+      <c r="E21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="9">
+      <c r="B22" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="8"/>
+      <c r="E22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="9">
+      <c r="B23" s="6">
         <v>10.3</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="8"/>
+      <c r="E23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="9">
+      <c r="B24" s="6">
         <v>10.4</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="8"/>
+      <c r="E24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="9">
+      <c r="B25" s="6">
         <v>11.1</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="8"/>
+      <c r="E25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="9">
+      <c r="B26" s="6">
         <v>11.2</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="8"/>
+      <c r="E26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="9">
+      <c r="B27" s="6">
         <v>12.1</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="8"/>
+      <c r="E27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="9">
+      <c r="B28" s="6">
         <v>12.2</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="8"/>
+      <c r="E28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="9">
+      <c r="B29" s="6">
         <v>15.1</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="8"/>
+      <c r="E29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="9">
+      <c r="B30" s="6">
         <v>15.2</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="8"/>
+      <c r="E30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="9">
+      <c r="B31" s="6">
         <v>18.100000000000001</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="8"/>
+      <c r="E31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="9">
+      <c r="B32" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="8"/>
+      <c r="E32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="9">
+      <c r="B33" s="6">
         <v>4.2</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="8"/>
+      <c r="E33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="9">
+      <c r="B34" s="6">
         <v>4.3</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="8"/>
+      <c r="E34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="9">
+      <c r="B35" s="6">
         <v>7.3</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="8"/>
+      <c r="E35" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="9">
+      <c r="B36" s="6">
         <v>8.1</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="8"/>
+      <c r="E36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="9">
+      <c r="B37" s="6">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="8"/>
+      <c r="E37" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="9">
+      <c r="B38" s="6">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F38" s="8"/>
+      <c r="E38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="9">
+      <c r="B39" s="6">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="8"/>
+      <c r="E39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="9">
+      <c r="B40" s="6">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" s="8"/>
+      <c r="E40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="9">
+      <c r="B41" s="6">
         <v>9.4</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F41" s="8"/>
+      <c r="E41" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="6"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="9">
+      <c r="B42" s="6">
         <v>13.1</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F42" s="8"/>
+      <c r="E42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="6"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="9">
+      <c r="B43" s="6">
         <v>13.2</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="8"/>
+      <c r="E43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="6"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="9">
+      <c r="B44" s="6">
         <v>14.1</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="8"/>
+      <c r="E44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="9">
+      <c r="B45" s="6">
         <v>14.2</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F45" s="8"/>
+      <c r="E45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="9">
+      <c r="B46" s="6">
         <v>16.100000000000001</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F46" s="8"/>
+      <c r="E46" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="6"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="9">
+      <c r="B47" s="6">
         <v>16.2</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" s="8"/>
+      <c r="E47" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="6"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="9">
+      <c r="B48" s="6">
         <v>17.100000000000001</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E48" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="8"/>
+      <c r="E48" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="6"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="9">
+      <c r="B49" s="6">
         <v>17.2</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F49" s="8"/>
+      <c r="E49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="6"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="9">
+      <c r="B50" s="6">
         <v>18.2</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E50" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F50" s="8"/>
+      <c r="E50" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="6"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="9">
+      <c r="B51" s="6">
         <v>19.100000000000001</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E51" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" s="8"/>
+      <c r="E51" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="6"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="9">
+      <c r="B52" s="6">
         <v>19.2</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F52" s="8"/>
+      <c r="E52" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="9">
+      <c r="B53" s="6">
         <v>20.100000000000001</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F53" s="8"/>
+      <c r="E53" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="6"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="9">
+      <c r="B54" s="6">
         <v>20.2</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E54" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="8"/>
+      <c r="E54" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:F54" xr:uid="{EDCC5412-150E-40F3-B8B9-815926E75632}">

</xml_diff>

<commit_message>
Remove Office temp file from index and update .gitignore
</commit_message>
<xml_diff>
--- a/doc/Road_To_Pro.xlsx
+++ b/doc/Road_To_Pro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE5C1B2-6FE9-4D62-9EC5-7990D5A1DFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD92A25-A8B9-4108-A704-7922395C37A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Entornos Segregados'!$B$2:$F$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -525,6 +526,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -532,9 +536,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -854,7 +855,7 @@
       <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -865,7 +866,7 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -874,7 +875,7 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -883,7 +884,7 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -892,7 +893,7 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
@@ -901,7 +902,7 @@
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -910,7 +911,7 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -919,21 +920,21 @@
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -942,14 +943,14 @@
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -958,7 +959,7 @@
       <c r="C15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="2:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
@@ -967,7 +968,7 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
@@ -976,7 +977,7 @@
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -987,7 +988,7 @@
       <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
@@ -996,7 +997,7 @@
       <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
@@ -1005,7 +1006,7 @@
       <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
@@ -1014,7 +1015,7 @@
       <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
@@ -1023,7 +1024,7 @@
       <c r="C22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
@@ -1032,7 +1033,7 @@
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
@@ -1041,7 +1042,7 @@
       <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1052,7 +1053,7 @@
       <c r="C25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
@@ -1061,7 +1062,7 @@
       <c r="C26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
@@ -1070,7 +1071,7 @@
       <c r="C27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
@@ -1079,7 +1080,7 @@
       <c r="C28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
@@ -1088,7 +1089,7 @@
       <c r="C29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1105,7 +1106,7 @@
   <dimension ref="B2:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,7 +1149,7 @@
       <c r="E3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1165,7 +1166,7 @@
       <c r="E4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
road to pro doc
</commit_message>
<xml_diff>
--- a/doc/Road_To_Pro.xlsx
+++ b/doc/Road_To_Pro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD92A25-A8B9-4108-A704-7922395C37A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FDCB13-E79A-4DD6-96AE-3E4CB4BA5D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Entornos Segregados'!$B$2:$F$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="131">
   <si>
     <t>Topic</t>
   </si>
@@ -1183,7 +1182,9 @@
       <c r="E5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="8" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="6">

</xml_diff>

<commit_message>
integrated new user_scheduler_runtime_status entitity into ingestion/publishing pipelines and in main modules
</commit_message>
<xml_diff>
--- a/doc/Road_To_Pro.xlsx
+++ b/doc/Road_To_Pro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FDCB13-E79A-4DD6-96AE-3E4CB4BA5D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0542663-92F8-4FBA-B4EB-C51C94C53D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -536,6 +536,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -820,16 +823,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" customWidth="1"/>
+    <col min="3" max="3" width="97.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1104,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCC5412-150E-40F3-B8B9-815926E75632}">
   <dimension ref="B2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1256,7 @@
       <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="12" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="6" t="s">

</xml_diff>

<commit_message>
minor fixes and minor changes in main and ingestion pipeline
</commit_message>
<xml_diff>
--- a/doc/Road_To_Pro.xlsx
+++ b/doc/Road_To_Pro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98551226-876F-46A7-86CF-1432FCBBFD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EED720-AF26-4C1F-8CBB-528CECBF7DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="139">
   <si>
     <t>Topic</t>
   </si>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F87B7-A3ED-42F6-8272-348ACF08162B}">
   <dimension ref="B1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1319,7 +1319,9 @@
       <c r="F19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="3">

</xml_diff>

<commit_message>
ingestion pipeline - added output language also in the user message
</commit_message>
<xml_diff>
--- a/doc/Road_To_Pro.xlsx
+++ b/doc/Road_To_Pro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software_projects\video2text\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EED720-AF26-4C1F-8CBB-528CECBF7DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C5899D-BEB5-44CF-8DB2-881CD4D2A3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tasks to PRO'!$B$2:$G$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -969,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F87B7-A3ED-42F6-8272-348ACF08162B}">
   <dimension ref="B1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>